<commit_message>
Amended bugs MWD,CPT and JobSummary
</commit_message>
<xml_diff>
--- a/assets/data/Summary/1633-SiteProgression.xlsx
+++ b/assets/data/Summary/1633-SiteProgression.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="859" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="991" uniqueCount="806">
   <si>
     <t>Time</t>
   </si>
@@ -139,6 +139,21 @@
     <t>3.4206 hr</t>
   </si>
   <si>
+    <t>2.2222 hr</t>
+  </si>
+  <si>
+    <t>1.6667 hr</t>
+  </si>
+  <si>
+    <t>3.2581 hr</t>
+  </si>
+  <si>
+    <t>2.6228 hr</t>
+  </si>
+  <si>
+    <t>1.4858 hr</t>
+  </si>
+  <si>
     <t>mean_MoveTime</t>
   </si>
   <si>
@@ -250,6 +265,21 @@
     <t>17.103 min</t>
   </si>
   <si>
+    <t>10.256 min</t>
+  </si>
+  <si>
+    <t>7.6923 min</t>
+  </si>
+  <si>
+    <t>17.771 min</t>
+  </si>
+  <si>
+    <t>13.114 min</t>
+  </si>
+  <si>
+    <t>8.915 min</t>
+  </si>
+  <si>
     <t>sum_DrillTime</t>
   </si>
   <si>
@@ -358,6 +388,21 @@
     <t>2.965 hr</t>
   </si>
   <si>
+    <t>2.9097 hr</t>
+  </si>
+  <si>
+    <t>3.155 hr</t>
+  </si>
+  <si>
+    <t>2.5622 hr</t>
+  </si>
+  <si>
+    <t>2.5231 hr</t>
+  </si>
+  <si>
+    <t>2.4811 hr</t>
+  </si>
+  <si>
     <t>mean_DrillTime</t>
   </si>
   <si>
@@ -466,6 +511,21 @@
     <t>13.685 min</t>
   </si>
   <si>
+    <t>12.47 min</t>
+  </si>
+  <si>
+    <t>13.521 min</t>
+  </si>
+  <si>
+    <t>12.811 min</t>
+  </si>
+  <si>
+    <t>11.645 min</t>
+  </si>
+  <si>
+    <t>13.533 min</t>
+  </si>
+  <si>
     <t>sum_GroutTime</t>
   </si>
   <si>
@@ -574,6 +634,21 @@
     <t>3.0178 hr</t>
   </si>
   <si>
+    <t>2.665 hr</t>
+  </si>
+  <si>
+    <t>2.7775 hr</t>
+  </si>
+  <si>
+    <t>2.9544 hr</t>
+  </si>
+  <si>
+    <t>2.2514 hr</t>
+  </si>
+  <si>
+    <t>2.3842 hr</t>
+  </si>
+  <si>
     <t>mean_GroutTime</t>
   </si>
   <si>
@@ -679,6 +754,21 @@
     <t>15.089 min</t>
   </si>
   <si>
+    <t>12.3 min</t>
+  </si>
+  <si>
+    <t>12.819 min</t>
+  </si>
+  <si>
+    <t>16.115 min</t>
+  </si>
+  <si>
+    <t>13.508 min</t>
+  </si>
+  <si>
+    <t>13.005 min</t>
+  </si>
+  <si>
     <t>sum_InstallTime</t>
   </si>
   <si>
@@ -784,6 +874,21 @@
     <t>7.0169 hr</t>
   </si>
   <si>
+    <t>6.7764 hr</t>
+  </si>
+  <si>
+    <t>6.9925 hr</t>
+  </si>
+  <si>
+    <t>6.0733 hr</t>
+  </si>
+  <si>
+    <t>6.5658 hr</t>
+  </si>
+  <si>
+    <t>5.3897 hr</t>
+  </si>
+  <si>
     <t>mean_InstallTime</t>
   </si>
   <si>
@@ -802,9 +907,6 @@
     <t>14.07 min</t>
   </si>
   <si>
-    <t>13.114 min</t>
-  </si>
-  <si>
     <t>15.61 min</t>
   </si>
   <si>
@@ -892,6 +994,21 @@
     <t>32.386 min</t>
   </si>
   <si>
+    <t>29.042 min</t>
+  </si>
+  <si>
+    <t>29.968 min</t>
+  </si>
+  <si>
+    <t>30.367 min</t>
+  </si>
+  <si>
+    <t>30.304 min</t>
+  </si>
+  <si>
+    <t>29.398 min</t>
+  </si>
+  <si>
     <t>sum_DelayTime</t>
   </si>
   <si>
@@ -1000,6 +1117,21 @@
     <t>2.4206 hr</t>
   </si>
   <si>
+    <t>1.1389 hr</t>
+  </si>
+  <si>
+    <t>0.59611 hr</t>
+  </si>
+  <si>
+    <t>2.3447 hr</t>
+  </si>
+  <si>
+    <t>1.6228 hr</t>
+  </si>
+  <si>
+    <t>0.68333 hr</t>
+  </si>
+  <si>
     <t>mean_DelayTime</t>
   </si>
   <si>
@@ -1108,6 +1240,21 @@
     <t>12.103 min</t>
   </si>
   <si>
+    <t>5.2564 min</t>
+  </si>
+  <si>
+    <t>2.7513 min</t>
+  </si>
+  <si>
+    <t>12.789 min</t>
+  </si>
+  <si>
+    <t>8.1139 min</t>
+  </si>
+  <si>
+    <t>4.1 min</t>
+  </si>
+  <si>
     <t>sum_CycleTime</t>
   </si>
   <si>
@@ -1216,6 +1363,21 @@
     <t>9.9628 hr</t>
   </si>
   <si>
+    <t>8.5089 hr</t>
+  </si>
+  <si>
+    <t>8.2161 hr</t>
+  </si>
+  <si>
+    <t>8.8669 hr</t>
+  </si>
+  <si>
+    <t>8.6333 hr</t>
+  </si>
+  <si>
+    <t>6.385 hr</t>
+  </si>
+  <si>
     <t>mean_CycleTime</t>
   </si>
   <si>
@@ -1324,6 +1486,21 @@
     <t>49.814 min</t>
   </si>
   <si>
+    <t>39.272 min</t>
+  </si>
+  <si>
+    <t>37.921 min</t>
+  </si>
+  <si>
+    <t>48.365 min</t>
+  </si>
+  <si>
+    <t>43.167 min</t>
+  </si>
+  <si>
+    <t>38.31 min</t>
+  </si>
+  <si>
     <t>sum_PileLength</t>
   </si>
   <si>
@@ -1444,6 +1621,21 @@
     <t>10.438 hr</t>
   </si>
   <si>
+    <t>8.9986 hr</t>
+  </si>
+  <si>
+    <t>8.6592 hr</t>
+  </si>
+  <si>
+    <t>9.3314 hr</t>
+  </si>
+  <si>
+    <t>9.1886 hr</t>
+  </si>
+  <si>
+    <t>6.8756 hr</t>
+  </si>
+  <si>
     <t>PileWaste</t>
   </si>
   <si>
@@ -1474,7 +1666,7 @@
     <t>11.5 hr</t>
   </si>
   <si>
-    <t>-2.5 hr</t>
+    <t>9.5 hr</t>
   </si>
   <si>
     <t>10.5 hr</t>
@@ -1486,9 +1678,6 @@
     <t>13 hr</t>
   </si>
   <si>
-    <t>-1 hr</t>
-  </si>
-  <si>
     <t>13.5 hr</t>
   </si>
   <si>
@@ -1618,6 +1807,21 @@
     <t>90.463 hr</t>
   </si>
   <si>
+    <t>92.686 hr</t>
+  </si>
+  <si>
+    <t>94.352 hr</t>
+  </si>
+  <si>
+    <t>97.61 hr</t>
+  </si>
+  <si>
+    <t>100.23 hr</t>
+  </si>
+  <si>
+    <t>101.72 hr</t>
+  </si>
+  <si>
     <t>HoursDrilled</t>
   </si>
   <si>
@@ -1723,6 +1927,21 @@
     <t>88.13 hr</t>
   </si>
   <si>
+    <t>91.04 hr</t>
+  </si>
+  <si>
+    <t>94.195 hr</t>
+  </si>
+  <si>
+    <t>96.757 hr</t>
+  </si>
+  <si>
+    <t>99.28 hr</t>
+  </si>
+  <si>
+    <t>101.76 hr</t>
+  </si>
+  <si>
     <t>HoursGrouted</t>
   </si>
   <si>
@@ -1828,6 +2047,21 @@
     <t>84.517 hr</t>
   </si>
   <si>
+    <t>87.182 hr</t>
+  </si>
+  <si>
+    <t>89.959 hr</t>
+  </si>
+  <si>
+    <t>92.914 hr</t>
+  </si>
+  <si>
+    <t>95.165 hr</t>
+  </si>
+  <si>
+    <t>97.549 hr</t>
+  </si>
+  <si>
     <t>HoursDelayed</t>
   </si>
   <si>
@@ -1933,6 +2167,21 @@
     <t>56.791 hr</t>
   </si>
   <si>
+    <t>57.93 hr</t>
+  </si>
+  <si>
+    <t>58.526 hr</t>
+  </si>
+  <si>
+    <t>60.871 hr</t>
+  </si>
+  <si>
+    <t>62.494 hr</t>
+  </si>
+  <si>
+    <t>63.177 hr</t>
+  </si>
+  <si>
     <t>HoursTurn</t>
   </si>
   <si>
@@ -2038,6 +2287,21 @@
     <t>284.19 hr</t>
   </si>
   <si>
+    <t>293.19 hr</t>
+  </si>
+  <si>
+    <t>301.85 hr</t>
+  </si>
+  <si>
+    <t>311.18 hr</t>
+  </si>
+  <si>
+    <t>320.37 hr</t>
+  </si>
+  <si>
+    <t>327.24 hr</t>
+  </si>
+  <si>
     <t>HoursCycle</t>
   </si>
   <si>
@@ -2141,6 +2405,21 @@
   </si>
   <si>
     <t>266.25 hr</t>
+  </si>
+  <si>
+    <t>274.76 hr</t>
+  </si>
+  <si>
+    <t>282.98 hr</t>
+  </si>
+  <si>
+    <t>291.84 hr</t>
+  </si>
+  <si>
+    <t>300.48 hr</t>
+  </si>
+  <si>
+    <t>306.86 hr</t>
   </si>
   <si>
     <t>DaysRigDrilled</t>
@@ -2198,7 +2477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD38"/>
+  <dimension ref="A1:AD44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2250,82 +2529,82 @@
         <v>4</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>221</v>
+        <v>251</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>256</v>
+        <v>291</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>292</v>
+        <v>331</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>328</v>
+        <v>372</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>364</v>
+        <v>413</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>400</v>
+        <v>454</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>436</v>
+        <v>495</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>437</v>
+        <v>496</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>438</v>
+        <v>497</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>439</v>
+        <v>498</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>440</v>
+        <v>499</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>441</v>
+        <v>500</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>476</v>
+        <v>540</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>477</v>
+        <v>541</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>478</v>
+        <v>542</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>479</v>
+        <v>543</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>480</v>
+        <v>544</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>481</v>
+        <v>545</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>482</v>
+        <v>546</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>483</v>
+        <v>547</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>498</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2">
@@ -2342,37 +2621,37 @@
         <v>5</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>257</v>
+        <v>292</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>293</v>
+        <v>332</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>329</v>
+        <v>373</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>365</v>
+        <v>414</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>401</v>
+        <v>455</v>
       </c>
       <c r="P2" s="0">
         <v>1005.6900000000001</v>
@@ -2390,7 +2669,7 @@
         <v>39.818402127995697</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>442</v>
+        <v>501</v>
       </c>
       <c r="V2" s="0">
         <v>1.1696853090760726</v>
@@ -2414,7 +2693,7 @@
         <v>45818.75</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD2" s="0">
         <v>1.2557008148964817</v>
@@ -2434,37 +2713,37 @@
         <v>6</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>258</v>
+        <v>293</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>294</v>
+        <v>333</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>366</v>
+        <v>415</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>402</v>
+        <v>456</v>
       </c>
       <c r="P3" s="0">
         <v>1955.6199999999997</v>
@@ -2482,7 +2761,7 @@
         <v>77.429092035866844</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>443</v>
+        <v>502</v>
       </c>
       <c r="V3" s="0">
         <v>1.1228337788040632</v>
@@ -2506,7 +2785,7 @@
         <v>45819.770833333336</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>485</v>
+        <v>549</v>
       </c>
       <c r="AD3" s="0">
         <v>1.1623538082857803</v>
@@ -2526,37 +2805,37 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>259</v>
+        <v>294</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>295</v>
+        <v>334</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>331</v>
+        <v>375</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>367</v>
+        <v>416</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>403</v>
+        <v>457</v>
       </c>
       <c r="P4" s="0">
         <v>1838.0299999999997</v>
@@ -2574,7 +2853,7 @@
         <v>72.773337373663779</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>444</v>
+        <v>503</v>
       </c>
       <c r="V4" s="0">
         <v>1.1624312289766452</v>
@@ -2598,7 +2877,7 @@
         <v>45820.75</v>
       </c>
       <c r="AC4" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD4" s="0">
         <v>1.1267863060747203</v>
@@ -2618,37 +2897,37 @@
         <v>8</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>260</v>
+        <v>295</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>332</v>
+        <v>376</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>368</v>
+        <v>417</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>404</v>
+        <v>458</v>
       </c>
       <c r="P5" s="0">
         <v>2067.6599999999999</v>
@@ -2666,7 +2945,7 @@
         <v>81.865104897107045</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>445</v>
+        <v>504</v>
       </c>
       <c r="V5" s="0">
         <v>1.1639757882160529</v>
@@ -2690,7 +2969,7 @@
         <v>45821.75</v>
       </c>
       <c r="AC5" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD5" s="0">
         <v>1.1237999403485905</v>
@@ -2710,37 +2989,37 @@
         <v>9</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>261</v>
+        <v>296</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>297</v>
+        <v>336</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>333</v>
+        <v>377</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>369</v>
+        <v>418</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>405</v>
+        <v>459</v>
       </c>
       <c r="P6" s="0">
         <v>1071.9200000000001</v>
@@ -2758,7 +3037,7 @@
         <v>42.440654286152935</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>446</v>
+        <v>505</v>
       </c>
       <c r="V6" s="0">
         <v>1.162446734853861</v>
@@ -2779,10 +3058,10 @@
         <v>45822.291666666664</v>
       </c>
       <c r="AB6" s="1">
-        <v>45822.1875</v>
+        <v>45822.6875</v>
       </c>
       <c r="AC6" s="0" t="s">
-        <v>486</v>
+        <v>550</v>
       </c>
       <c r="AD6" s="0">
         <v>1.1781156733088689</v>
@@ -2802,37 +3081,37 @@
         <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>262</v>
+        <v>86</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>298</v>
+        <v>337</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>334</v>
+        <v>378</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>370</v>
+        <v>419</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>406</v>
+        <v>460</v>
       </c>
       <c r="P7" s="0">
         <v>2068.3699999999999</v>
@@ -2850,7 +3129,7 @@
         <v>81.893216010383355</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>447</v>
+        <v>506</v>
       </c>
       <c r="V7" s="0">
         <v>1.1644187961541217</v>
@@ -2874,7 +3153,7 @@
         <v>45824.729166666664</v>
       </c>
       <c r="AC7" s="0" t="s">
-        <v>487</v>
+        <v>551</v>
       </c>
       <c r="AD7" s="0">
         <v>1.1600472496763934</v>
@@ -2894,37 +3173,37 @@
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>299</v>
+        <v>338</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>335</v>
+        <v>379</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>371</v>
+        <v>420</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>407</v>
+        <v>461</v>
       </c>
       <c r="P8" s="0">
         <v>1071.9200000000001</v>
@@ -2942,7 +3221,7 @@
         <v>42.440654286152942</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>448</v>
+        <v>507</v>
       </c>
       <c r="V8" s="0">
         <v>1.2014659259538503</v>
@@ -2966,7 +3245,7 @@
         <v>45825.708333333336</v>
       </c>
       <c r="AC8" s="0" t="s">
-        <v>488</v>
+        <v>552</v>
       </c>
       <c r="AD8" s="0">
         <v>1.1545533598426914</v>
@@ -2986,37 +3265,37 @@
         <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>264</v>
+        <v>298</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>300</v>
+        <v>339</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>336</v>
+        <v>380</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>372</v>
+        <v>421</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>408</v>
+        <v>462</v>
       </c>
       <c r="P9" s="0">
         <v>1445.6899999999998</v>
@@ -3034,7 +3313,7 @@
         <v>94.620189236838073</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>449</v>
+        <v>508</v>
       </c>
       <c r="V9" s="0">
         <v>1.1164530619948498</v>
@@ -3058,7 +3337,7 @@
         <v>45827.75</v>
       </c>
       <c r="AC9" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD9" s="0">
         <v>1.1836797294883818</v>
@@ -3078,37 +3357,37 @@
         <v>13</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>265</v>
+        <v>299</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>301</v>
+        <v>340</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>337</v>
+        <v>381</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>373</v>
+        <v>422</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>409</v>
+        <v>463</v>
       </c>
       <c r="P10" s="0">
         <v>1630.8099999999999</v>
@@ -3126,7 +3405,7 @@
         <v>106.73626490418272</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>450</v>
+        <v>509</v>
       </c>
       <c r="V10" s="0">
         <v>1.1267679275451865</v>
@@ -3150,7 +3429,7 @@
         <v>45828.708333333336</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD10" s="0">
         <v>1.1430042086400489</v>
@@ -3170,37 +3449,37 @@
         <v>14</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>302</v>
+        <v>341</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>338</v>
+        <v>382</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>374</v>
+        <v>423</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>410</v>
+        <v>464</v>
       </c>
       <c r="P11" s="0">
         <v>1446.5899999999997</v>
@@ -3218,7 +3497,7 @@
         <v>94.679094099092893</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>451</v>
+        <v>510</v>
       </c>
       <c r="V11" s="0">
         <v>1.1332491192586092</v>
@@ -3242,7 +3521,7 @@
         <v>45831.770833333336</v>
       </c>
       <c r="AC11" s="0" t="s">
-        <v>485</v>
+        <v>549</v>
       </c>
       <c r="AD11" s="0">
         <v>1.172381306097261</v>
@@ -3262,37 +3541,37 @@
         <v>15</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>267</v>
+        <v>301</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>303</v>
+        <v>342</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>339</v>
+        <v>383</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>375</v>
+        <v>424</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>411</v>
+        <v>465</v>
       </c>
       <c r="P12" s="0">
         <v>1583.1600000000001</v>
@@ -3310,7 +3589,7 @@
         <v>103.61757969702535</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>452</v>
+        <v>511</v>
       </c>
       <c r="V12" s="0">
         <v>1.1380404786986671</v>
@@ -3334,7 +3613,7 @@
         <v>45832.6875</v>
       </c>
       <c r="AC12" s="0" t="s">
-        <v>488</v>
+        <v>552</v>
       </c>
       <c r="AD12" s="0">
         <v>0.11581046416146405</v>
@@ -3354,37 +3633,37 @@
         <v>16</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>268</v>
+        <v>302</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>304</v>
+        <v>343</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>340</v>
+        <v>384</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>376</v>
+        <v>425</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>412</v>
+        <v>466</v>
       </c>
       <c r="P13" s="0">
         <v>1584.28</v>
@@ -3402,7 +3681,7 @@
         <v>103.69088352560911</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>453</v>
+        <v>512</v>
       </c>
       <c r="V13" s="0">
         <v>1.1425594610806848</v>
@@ -3426,7 +3705,7 @@
         <v>45833.6875</v>
       </c>
       <c r="AC13" s="0" t="s">
-        <v>488</v>
+        <v>552</v>
       </c>
       <c r="AD13" s="0">
         <v>1.186218072581299</v>
@@ -3446,37 +3725,37 @@
         <v>17</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>269</v>
+        <v>303</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>305</v>
+        <v>344</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>341</v>
+        <v>385</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>377</v>
+        <v>426</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>413</v>
+        <v>467</v>
       </c>
       <c r="P14" s="0">
         <v>1583.2899999999995</v>
@@ -3494,7 +3773,7 @@
         <v>103.62608817712881</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>394</v>
+        <v>443</v>
       </c>
       <c r="V14" s="0">
         <v>1.1406104589991377</v>
@@ -3518,7 +3797,7 @@
         <v>45834.791666666664</v>
       </c>
       <c r="AC14" s="0" t="s">
-        <v>489</v>
+        <v>553</v>
       </c>
       <c r="AD14" s="0">
         <v>1.1773097117346023</v>
@@ -3538,37 +3817,37 @@
         <v>18</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>270</v>
+        <v>304</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>306</v>
+        <v>345</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>342</v>
+        <v>386</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>378</v>
+        <v>427</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>414</v>
+        <v>468</v>
       </c>
       <c r="P15" s="0">
         <v>1386.1299999999999</v>
@@ -3586,7 +3865,7 @@
         <v>90.721996352508768</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>454</v>
+        <v>513</v>
       </c>
       <c r="V15" s="0">
         <v>1.138566214952385</v>
@@ -3610,7 +3889,7 @@
         <v>45835.75</v>
       </c>
       <c r="AC15" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD15" s="0">
         <v>1.1353365682098078</v>
@@ -3630,37 +3909,37 @@
         <v>19</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>271</v>
+        <v>305</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>307</v>
+        <v>346</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>343</v>
+        <v>387</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>379</v>
+        <v>428</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>415</v>
+        <v>469</v>
       </c>
       <c r="P16" s="0">
         <v>1450.2899999999997</v>
@@ -3678,7 +3957,7 @@
         <v>94.921258532807101</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>455</v>
+        <v>514</v>
       </c>
       <c r="V16" s="0">
         <v>1.1405348145756238</v>
@@ -3702,7 +3981,7 @@
         <v>45838.729166666664</v>
       </c>
       <c r="AC16" s="0" t="s">
-        <v>487</v>
+        <v>551</v>
       </c>
       <c r="AD16" s="0">
         <v>1.2852758368962609</v>
@@ -3722,37 +4001,37 @@
         <v>20</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>272</v>
+        <v>306</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>308</v>
+        <v>347</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>344</v>
+        <v>388</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>380</v>
+        <v>429</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>416</v>
+        <v>470</v>
       </c>
       <c r="P17" s="0">
         <v>1585.0899999999999</v>
@@ -3770,7 +4049,7 @@
         <v>103.74389790163845</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>456</v>
+        <v>515</v>
       </c>
       <c r="V17" s="0">
         <v>1.1373199039799773</v>
@@ -3791,10 +4070,10 @@
         <v>45839.25</v>
       </c>
       <c r="AB17" s="1">
-        <v>45839.208333333336</v>
+        <v>45839.708333333336</v>
       </c>
       <c r="AC17" s="0" t="s">
-        <v>490</v>
+        <v>548</v>
       </c>
       <c r="AD17" s="0">
         <v>1.1759727797741946</v>
@@ -3814,37 +4093,37 @@
         <v>21</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>237</v>
+        <v>267</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>309</v>
+        <v>348</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>345</v>
+        <v>389</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>381</v>
+        <v>430</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>417</v>
+        <v>471</v>
       </c>
       <c r="P18" s="0">
         <v>1581.0699999999997</v>
@@ -3862,7 +4141,7 @@
         <v>103.4807895169003</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>457</v>
+        <v>516</v>
       </c>
       <c r="V18" s="0">
         <v>1.1408784234364466</v>
@@ -3886,7 +4165,7 @@
         <v>45840.708333333336</v>
       </c>
       <c r="AC18" s="0" t="s">
-        <v>488</v>
+        <v>552</v>
       </c>
       <c r="AD18" s="0">
         <v>1.1789627869052466</v>
@@ -3906,37 +4185,37 @@
         <v>22</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>238</v>
+        <v>268</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>310</v>
+        <v>349</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>346</v>
+        <v>390</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>382</v>
+        <v>431</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>418</v>
+        <v>472</v>
       </c>
       <c r="P19" s="0">
         <v>663.74000000000001</v>
@@ -3954,7 +4233,7 @@
         <v>43.441681414451857</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>458</v>
+        <v>517</v>
       </c>
       <c r="V19" s="0">
         <v>1.1420138075847079</v>
@@ -3978,7 +4257,7 @@
         <v>45852.854166666664</v>
       </c>
       <c r="AC19" s="0" t="s">
-        <v>491</v>
+        <v>554</v>
       </c>
       <c r="AD19" s="0">
         <v>2.0717430143037574</v>
@@ -3998,37 +4277,37 @@
         <v>23</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>275</v>
+        <v>309</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>311</v>
+        <v>350</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>347</v>
+        <v>391</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>383</v>
+        <v>432</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>419</v>
+        <v>473</v>
       </c>
       <c r="P20" s="0">
         <v>924.24999999999977</v>
@@ -4046,7 +4325,7 @@
         <v>60.492021043340962</v>
       </c>
       <c r="U20" s="0" t="s">
-        <v>459</v>
+        <v>518</v>
       </c>
       <c r="V20" s="0">
         <v>1.1509121169900798</v>
@@ -4070,7 +4349,7 @@
         <v>45853.75</v>
       </c>
       <c r="AC20" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD20" s="0">
         <v>1.2398329350951003</v>
@@ -4090,37 +4369,37 @@
         <v>24</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>276</v>
+        <v>310</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>312</v>
+        <v>351</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>348</v>
+        <v>392</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>384</v>
+        <v>433</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>420</v>
+        <v>474</v>
       </c>
       <c r="P21" s="0">
         <v>1718.8499999999999</v>
@@ -4138,7 +4417,7 @@
         <v>112.498469429642</v>
       </c>
       <c r="U21" s="0" t="s">
-        <v>460</v>
+        <v>519</v>
       </c>
       <c r="V21" s="0">
         <v>1.1444955709421847</v>
@@ -4162,7 +4441,7 @@
         <v>45854.771527777775</v>
       </c>
       <c r="AC21" s="0" t="s">
-        <v>492</v>
+        <v>555</v>
       </c>
       <c r="AD21" s="0">
         <v>1.2800174147263352</v>
@@ -4182,37 +4461,37 @@
         <v>25</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>277</v>
+        <v>311</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>313</v>
+        <v>352</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>349</v>
+        <v>393</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>385</v>
+        <v>434</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>421</v>
+        <v>475</v>
       </c>
       <c r="P22" s="0">
         <v>1588.8299999999999</v>
@@ -4230,7 +4509,7 @@
         <v>103.98868032923065</v>
       </c>
       <c r="U22" s="0" t="s">
-        <v>461</v>
+        <v>520</v>
       </c>
       <c r="V22" s="0">
         <v>1.1333156611554043</v>
@@ -4254,7 +4533,7 @@
         <v>45855.854166666664</v>
       </c>
       <c r="AC22" s="0" t="s">
-        <v>493</v>
+        <v>556</v>
       </c>
       <c r="AD22" s="0">
         <v>1.1732046181732962</v>
@@ -4274,37 +4553,37 @@
         <v>26</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>314</v>
+        <v>353</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>386</v>
+        <v>435</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>422</v>
+        <v>476</v>
       </c>
       <c r="P23" s="0">
         <v>1584.3199999999997</v>
@@ -4322,7 +4601,7 @@
         <v>103.6935015194871</v>
       </c>
       <c r="U23" s="0" t="s">
-        <v>462</v>
+        <v>521</v>
       </c>
       <c r="V23" s="0">
         <v>1.1591661795451205</v>
@@ -4346,7 +4625,7 @@
         <v>45856.833333333336</v>
       </c>
       <c r="AC23" s="0" t="s">
-        <v>491</v>
+        <v>554</v>
       </c>
       <c r="AD23" s="0">
         <v>1.4658584942416537</v>
@@ -4366,37 +4645,37 @@
         <v>27</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>279</v>
+        <v>313</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>315</v>
+        <v>354</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>351</v>
+        <v>395</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>387</v>
+        <v>436</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>423</v>
+        <v>477</v>
       </c>
       <c r="P24" s="0">
         <v>1057.6699999999998</v>
@@ -4414,7 +4693,7 @@
         <v>69.224339623381582</v>
       </c>
       <c r="U24" s="0" t="s">
-        <v>463</v>
+        <v>522</v>
       </c>
       <c r="V24" s="0">
         <v>1.1751791413626207</v>
@@ -4438,7 +4717,7 @@
         <v>45857.583333333336</v>
       </c>
       <c r="AC24" s="0" t="s">
-        <v>494</v>
+        <v>557</v>
       </c>
       <c r="AD24" s="0">
         <v>1.184554456512334</v>
@@ -4458,37 +4737,37 @@
         <v>28</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>316</v>
+        <v>355</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>352</v>
+        <v>396</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>388</v>
+        <v>437</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>424</v>
+        <v>478</v>
       </c>
       <c r="P25" s="0">
         <v>1851.9599999999998</v>
@@ -4506,7 +4785,7 @@
         <v>121.2104985571282</v>
       </c>
       <c r="U25" s="0" t="s">
-        <v>464</v>
+        <v>523</v>
       </c>
       <c r="V25" s="0">
         <v>1.1886099118064173</v>
@@ -4530,7 +4809,7 @@
         <v>45859.791666666664</v>
       </c>
       <c r="AC25" s="0" t="s">
-        <v>495</v>
+        <v>558</v>
       </c>
       <c r="AD25" s="0">
         <v>1.2210163456282257</v>
@@ -4550,37 +4829,37 @@
         <v>29</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>281</v>
+        <v>315</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>317</v>
+        <v>356</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>353</v>
+        <v>397</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>389</v>
+        <v>438</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>425</v>
+        <v>479</v>
       </c>
       <c r="P26" s="0">
         <v>933.63999999999999</v>
@@ -4598,7 +4877,7 @@
         <v>61.106595106199471</v>
       </c>
       <c r="U26" s="0" t="s">
-        <v>465</v>
+        <v>524</v>
       </c>
       <c r="V26" s="0">
         <v>1.1449827940569008</v>
@@ -4622,7 +4901,7 @@
         <v>45860.895833333336</v>
       </c>
       <c r="AC26" s="0" t="s">
-        <v>496</v>
+        <v>559</v>
       </c>
       <c r="AD26" s="0">
         <v>1.6692142611240297</v>
@@ -4640,37 +4919,37 @@
         <v>30</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>30</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="J27" s="0" t="s">
         <v>30</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="L27" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="N27" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="P27" s="0"/>
       <c r="Q27" s="0"/>
@@ -4708,37 +4987,37 @@
         <v>31</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>282</v>
+        <v>316</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>318</v>
+        <v>357</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>354</v>
+        <v>398</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>390</v>
+        <v>439</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>426</v>
+        <v>480</v>
       </c>
       <c r="P28" s="0">
         <v>1339.1999999999998</v>
@@ -4756,7 +5035,7 @@
         <v>87.650435035155226</v>
       </c>
       <c r="U28" s="0" t="s">
-        <v>466</v>
+        <v>525</v>
       </c>
       <c r="V28" s="0">
         <v>1.1351683532442582</v>
@@ -4780,7 +5059,7 @@
         <v>45863.729166666664</v>
       </c>
       <c r="AC28" s="0" t="s">
-        <v>485</v>
+        <v>549</v>
       </c>
       <c r="AD28" s="0">
         <v>1.2778031273327799</v>
@@ -4800,37 +5079,37 @@
         <v>32</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>283</v>
+        <v>317</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>319</v>
+        <v>358</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>355</v>
+        <v>399</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>391</v>
+        <v>440</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>427</v>
+        <v>481</v>
       </c>
       <c r="P29" s="0">
         <v>1720.7099999999996</v>
@@ -4848,7 +5127,7 @@
         <v>112.62020614496859</v>
       </c>
       <c r="U29" s="0" t="s">
-        <v>467</v>
+        <v>526</v>
       </c>
       <c r="V29" s="0">
         <v>1.1297794983274803</v>
@@ -4872,7 +5151,7 @@
         <v>45864.75</v>
       </c>
       <c r="AC29" s="0" t="s">
-        <v>485</v>
+        <v>549</v>
       </c>
       <c r="AD29" s="0">
         <v>1.1454427621447147</v>
@@ -4892,37 +5171,37 @@
         <v>33</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>248</v>
+        <v>278</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>284</v>
+        <v>318</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>320</v>
+        <v>359</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>356</v>
+        <v>400</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>392</v>
+        <v>441</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>428</v>
+        <v>482</v>
       </c>
       <c r="P30" s="0">
         <v>1739.2999999999997</v>
@@ -4940,7 +5219,7 @@
         <v>113.83691879976516</v>
       </c>
       <c r="U30" s="0" t="s">
-        <v>468</v>
+        <v>527</v>
       </c>
       <c r="V30" s="0">
         <v>1.1352819574054267</v>
@@ -4964,7 +5243,7 @@
         <v>45866.75</v>
       </c>
       <c r="AC30" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD30" s="0">
         <v>1.1332000317656712</v>
@@ -4984,37 +5263,37 @@
         <v>34</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>214</v>
+        <v>239</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>249</v>
+        <v>279</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>285</v>
+        <v>319</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>357</v>
+        <v>401</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>393</v>
+        <v>442</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>429</v>
+        <v>483</v>
       </c>
       <c r="P31" s="0">
         <v>1726.3699999999997</v>
@@ -5032,7 +5311,7 @@
         <v>112.9906522787044</v>
       </c>
       <c r="U31" s="0" t="s">
-        <v>469</v>
+        <v>528</v>
       </c>
       <c r="V31" s="0">
         <v>1.1175260736484693</v>
@@ -5056,7 +5335,7 @@
         <v>45867.770833333336</v>
       </c>
       <c r="AC31" s="0" t="s">
-        <v>497</v>
+        <v>560</v>
       </c>
       <c r="AD31" s="0">
         <v>1.1151364954439464</v>
@@ -5076,37 +5355,37 @@
         <v>35</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>286</v>
+        <v>320</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>322</v>
+        <v>361</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>358</v>
+        <v>402</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>394</v>
+        <v>443</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>430</v>
+        <v>484</v>
       </c>
       <c r="P32" s="0">
         <v>1199.3999999999999</v>
@@ -5124,7 +5403,7 @@
         <v>78.500546431574961</v>
       </c>
       <c r="U32" s="0" t="s">
-        <v>470</v>
+        <v>529</v>
       </c>
       <c r="V32" s="0">
         <v>1.1417882304568021</v>
@@ -5148,7 +5427,7 @@
         <v>45868.729166666664</v>
       </c>
       <c r="AC32" s="0" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="AD32" s="0">
         <v>1.171966364338519</v>
@@ -5168,37 +5447,37 @@
         <v>36</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>287</v>
+        <v>321</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>323</v>
+        <v>362</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>359</v>
+        <v>403</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>395</v>
+        <v>444</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>431</v>
+        <v>485</v>
       </c>
       <c r="P33" s="0">
         <v>1230.2199999999998</v>
@@ -5216,7 +5495,7 @@
         <v>80.517710714567386</v>
       </c>
       <c r="U33" s="0" t="s">
-        <v>471</v>
+        <v>530</v>
       </c>
       <c r="V33" s="0">
         <v>1.1620300573582039</v>
@@ -5240,7 +5519,7 @@
         <v>45869.75</v>
       </c>
       <c r="AC33" s="0" t="s">
-        <v>485</v>
+        <v>549</v>
       </c>
       <c r="AD33" s="0">
         <v>1.1426057594475947</v>
@@ -5260,37 +5539,37 @@
         <v>37</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>252</v>
+        <v>282</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>324</v>
+        <v>363</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>360</v>
+        <v>404</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>396</v>
+        <v>445</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>432</v>
+        <v>486</v>
       </c>
       <c r="P34" s="0">
         <v>1728.6299999999999</v>
@@ -5308,7 +5587,7 @@
         <v>113.13856893281093</v>
       </c>
       <c r="U34" s="0" t="s">
-        <v>472</v>
+        <v>531</v>
       </c>
       <c r="V34" s="0">
         <v>1.1435092490592784</v>
@@ -5332,7 +5611,7 @@
         <v>45870.75</v>
       </c>
       <c r="AC34" s="0" t="s">
-        <v>485</v>
+        <v>549</v>
       </c>
       <c r="AD34" s="0">
         <v>1.1136785729968621</v>
@@ -5350,37 +5629,37 @@
         <v>30</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>30</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>30</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="J35" s="0" t="s">
         <v>30</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="L35" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="N35" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="P35" s="0"/>
       <c r="Q35" s="0"/>
@@ -5418,37 +5697,37 @@
         <v>38</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>253</v>
+        <v>283</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>289</v>
+        <v>323</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>325</v>
+        <v>364</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>361</v>
+        <v>405</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>397</v>
+        <v>446</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>433</v>
+        <v>487</v>
       </c>
       <c r="P36" s="0">
         <v>2001.0499999999995</v>
@@ -5466,7 +5745,7 @@
         <v>130.96841623887198</v>
       </c>
       <c r="U36" s="0" t="s">
-        <v>473</v>
+        <v>532</v>
       </c>
       <c r="V36" s="0">
         <v>1.1421990453573223</v>
@@ -5490,7 +5769,7 @@
         <v>45873.833333333336</v>
       </c>
       <c r="AC36" s="0" t="s">
-        <v>491</v>
+        <v>554</v>
       </c>
       <c r="AD36" s="0">
         <v>1.1605851575907333</v>
@@ -5510,37 +5789,37 @@
         <v>39</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>254</v>
+        <v>284</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>290</v>
+        <v>324</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="M37" s="0" t="s">
-        <v>362</v>
+        <v>406</v>
       </c>
       <c r="N37" s="0" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>434</v>
+        <v>488</v>
       </c>
       <c r="P37" s="0">
         <v>1793.8199999999997</v>
@@ -5558,7 +5837,7 @@
         <v>117.40524445546755</v>
       </c>
       <c r="U37" s="0" t="s">
-        <v>474</v>
+        <v>533</v>
       </c>
       <c r="V37" s="0">
         <v>1.1442674526431145</v>
@@ -5582,7 +5861,7 @@
         <v>45874.75</v>
       </c>
       <c r="AC37" s="0" t="s">
-        <v>485</v>
+        <v>549</v>
       </c>
       <c r="AD37" s="0">
         <v>1.0902409052821409</v>
@@ -5602,37 +5881,37 @@
         <v>40</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>255</v>
+        <v>285</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>291</v>
+        <v>325</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>327</v>
+        <v>366</v>
       </c>
       <c r="M38" s="0" t="s">
-        <v>363</v>
+        <v>407</v>
       </c>
       <c r="N38" s="0" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
       <c r="O38" s="0" t="s">
-        <v>435</v>
+        <v>489</v>
       </c>
       <c r="P38" s="0">
         <v>1743.9399999999998</v>
@@ -5650,16 +5929,16 @@
         <v>114.14060608961216</v>
       </c>
       <c r="U38" s="0" t="s">
-        <v>475</v>
+        <v>534</v>
       </c>
       <c r="V38" s="0">
         <v>1.1189619923669183</v>
       </c>
       <c r="W38" s="0">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="X38" s="0">
-        <v>0</v>
+        <v>94.5</v>
       </c>
       <c r="Y38" s="1">
         <v>45875.298750000002</v>
@@ -5667,13 +5946,543 @@
       <c r="Z38" s="1">
         <v>45875.73364583333</v>
       </c>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
+      <c r="AA38" s="1">
+        <v>45875.270833333336</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>45875.770833333336</v>
+      </c>
       <c r="AC38" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="AD38" s="0">
+        <v>1.1214238682025814</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1">
+        <v>45876</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="0">
+        <v>14</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="N39" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="P39" s="0">
+        <v>1924.5899999999999</v>
+      </c>
+      <c r="Q39" s="0">
+        <v>137.47071428571428</v>
+      </c>
+      <c r="R39" s="0">
+        <v>1.1253599807568555</v>
+      </c>
+      <c r="S39" s="0">
+        <v>141.726</v>
+      </c>
+      <c r="T39" s="0">
+        <v>125.96412094109127</v>
+      </c>
+      <c r="U39" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="V39" s="0">
+        <v>1.1251299095420988</v>
+      </c>
+      <c r="W39" s="0">
+        <v>137</v>
+      </c>
+      <c r="X39" s="0">
+        <v>87</v>
+      </c>
+      <c r="Y39" s="1">
+        <v>45876.30541666667</v>
+      </c>
+      <c r="Z39" s="1">
+        <v>45876.680358796293</v>
+      </c>
+      <c r="AA39" s="1">
+        <v>45876.270833333336</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>45876.729166666664</v>
+      </c>
+      <c r="AC39" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="AD39" s="0">
+        <v>1.0876112894406638</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1">
+        <v>45877</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="0">
+        <v>14</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="N40" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="O40" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="P40" s="0">
+        <v>1904.8199999999999</v>
+      </c>
+      <c r="Q40" s="0">
+        <v>136.05857142857141</v>
+      </c>
+      <c r="R40" s="0">
+        <v>1.1129284947571054</v>
+      </c>
+      <c r="S40" s="0">
+        <v>138.75899999999999</v>
+      </c>
+      <c r="T40" s="0">
+        <v>124.67017746689395</v>
+      </c>
+      <c r="U40" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="V40" s="0">
+        <v>1.1130087629565404</v>
+      </c>
+      <c r="W40" s="0">
+        <v>136</v>
+      </c>
+      <c r="X40" s="0">
+        <v>80</v>
+      </c>
+      <c r="Y40" s="1">
+        <v>45877.303587962961</v>
+      </c>
+      <c r="Z40" s="1">
+        <v>45877.664386574077</v>
+      </c>
+      <c r="AA40" s="1">
+        <v>45877.270833333336</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>45877.708333333336</v>
+      </c>
+      <c r="AC40" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="AD40" s="0">
+        <v>1.0908783701387983</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1">
+        <v>45878</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="AD38" s="0">
+      <c r="E41" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="N41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O41" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="P41" s="0"/>
+      <c r="Q41" s="0"/>
+      <c r="R41" s="0"/>
+      <c r="S41" s="0"/>
+      <c r="T41" s="0"/>
+      <c r="U41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="V41" s="0"/>
+      <c r="W41" s="0"/>
+      <c r="X41" s="0">
         <v>0</v>
+      </c>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD41" s="0"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1">
+        <v>45880</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="0">
+        <v>12</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="N42" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="O42" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="P42" s="0">
+        <v>1594.9899999999998</v>
+      </c>
+      <c r="Q42" s="0">
+        <v>132.91583333333332</v>
+      </c>
+      <c r="R42" s="0">
+        <v>1.1467383804143929</v>
+      </c>
+      <c r="S42" s="0">
+        <v>119.71500000000002</v>
+      </c>
+      <c r="T42" s="0">
+        <v>104.39185138644132</v>
+      </c>
+      <c r="U42" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="V42" s="0">
+        <v>1.1467849109873045</v>
+      </c>
+      <c r="W42" s="0">
+        <v>122</v>
+      </c>
+      <c r="X42" s="0">
+        <v>90.5</v>
+      </c>
+      <c r="Y42" s="1">
+        <v>45880.301898148151</v>
+      </c>
+      <c r="Z42" s="1">
+        <v>45880.690706018519</v>
+      </c>
+      <c r="AA42" s="1">
+        <v>45880.270833333336</v>
+      </c>
+      <c r="AB42" s="1">
+        <v>45880.75</v>
+      </c>
+      <c r="AC42" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="AD42" s="0">
+        <v>1.1686735926195642</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>45881</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="0">
+        <v>13</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="N43" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="O43" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="P43" s="0">
+        <v>1779.2799999999997</v>
+      </c>
+      <c r="Q43" s="0">
+        <v>136.86769230769229</v>
+      </c>
+      <c r="R43" s="0">
+        <v>1.1175234013522484</v>
+      </c>
+      <c r="S43" s="0">
+        <v>130.13400000000001</v>
+      </c>
+      <c r="T43" s="0">
+        <v>116.45360368081765</v>
+      </c>
+      <c r="U43" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="V43" s="0">
+        <v>1.1174750792313679</v>
+      </c>
+      <c r="W43" s="0">
+        <v>128</v>
+      </c>
+      <c r="X43" s="0">
+        <v>90.5</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>45881.300752314812</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>45881.683611111112</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>45881.270833333336</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>45881.75</v>
+      </c>
+      <c r="AC43" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="AD43" s="0">
+        <v>1.0991501847450711</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1">
+        <v>45882</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="0">
+        <v>11</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="M44" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="N44" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="O44" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="P44" s="0">
+        <v>1466.3200000000002</v>
+      </c>
+      <c r="Q44" s="0">
+        <v>133.30181818181819</v>
+      </c>
+      <c r="R44" s="0">
+        <v>1.1129680893216005</v>
+      </c>
+      <c r="S44" s="0">
+        <v>106.812</v>
+      </c>
+      <c r="T44" s="0">
+        <v>95.970419579412194</v>
+      </c>
+      <c r="U44" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="V44" s="0">
+        <v>1.1129679381219832</v>
+      </c>
+      <c r="W44" s="0">
+        <v>128</v>
+      </c>
+      <c r="X44" s="0">
+        <v>83.5</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>45882.304351851853</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>45882.590833333335</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>45882.25</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>45882.729166666664</v>
+      </c>
+      <c r="AC44" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="AD44" s="0">
+        <v>1.3337442991388033</v>
       </c>
     </row>
   </sheetData>
@@ -5682,7 +6491,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5716,40 +6525,40 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>499</v>
+        <v>562</v>
       </c>
       <c r="E1" t="s">
-        <v>534</v>
+        <v>602</v>
       </c>
       <c r="F1" t="s">
-        <v>569</v>
+        <v>642</v>
       </c>
       <c r="G1" t="s">
-        <v>604</v>
+        <v>682</v>
       </c>
       <c r="H1" t="s">
-        <v>639</v>
+        <v>722</v>
       </c>
       <c r="I1" t="s">
-        <v>674</v>
+        <v>762</v>
       </c>
       <c r="J1" t="s">
-        <v>709</v>
+        <v>802</v>
       </c>
       <c r="K1" t="s">
-        <v>710</v>
+        <v>803</v>
       </c>
       <c r="L1" t="s">
-        <v>711</v>
+        <v>804</v>
       </c>
       <c r="M1" t="s">
-        <v>712</v>
+        <v>805</v>
       </c>
       <c r="N1" t="s">
-        <v>477</v>
+        <v>541</v>
       </c>
       <c r="O1" t="s">
-        <v>478</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2">
@@ -5766,19 +6575,19 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="G2" t="s">
-        <v>293</v>
+        <v>332</v>
       </c>
       <c r="H2" t="s">
-        <v>442</v>
+        <v>501</v>
       </c>
       <c r="I2" t="s">
-        <v>365</v>
+        <v>414</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -5810,22 +6619,22 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>500</v>
+        <v>563</v>
       </c>
       <c r="E3" t="s">
-        <v>535</v>
+        <v>603</v>
       </c>
       <c r="F3" t="s">
-        <v>570</v>
+        <v>643</v>
       </c>
       <c r="G3" t="s">
-        <v>605</v>
+        <v>683</v>
       </c>
       <c r="H3" t="s">
-        <v>640</v>
+        <v>723</v>
       </c>
       <c r="I3" t="s">
-        <v>675</v>
+        <v>763</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -5857,22 +6666,22 @@
         <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>501</v>
+        <v>564</v>
       </c>
       <c r="E4" t="s">
-        <v>536</v>
+        <v>604</v>
       </c>
       <c r="F4" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
       <c r="G4" t="s">
-        <v>606</v>
+        <v>684</v>
       </c>
       <c r="H4" t="s">
-        <v>641</v>
+        <v>724</v>
       </c>
       <c r="I4" t="s">
-        <v>676</v>
+        <v>764</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -5904,22 +6713,22 @@
         <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>502</v>
+        <v>565</v>
       </c>
       <c r="E5" t="s">
-        <v>537</v>
+        <v>605</v>
       </c>
       <c r="F5" t="s">
-        <v>572</v>
+        <v>645</v>
       </c>
       <c r="G5" t="s">
-        <v>607</v>
+        <v>685</v>
       </c>
       <c r="H5" t="s">
-        <v>642</v>
+        <v>725</v>
       </c>
       <c r="I5" t="s">
-        <v>677</v>
+        <v>765</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -5951,22 +6760,22 @@
         <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>503</v>
+        <v>566</v>
       </c>
       <c r="E6" t="s">
-        <v>538</v>
+        <v>606</v>
       </c>
       <c r="F6" t="s">
-        <v>573</v>
+        <v>646</v>
       </c>
       <c r="G6" t="s">
-        <v>608</v>
+        <v>686</v>
       </c>
       <c r="H6" t="s">
-        <v>643</v>
+        <v>726</v>
       </c>
       <c r="I6" t="s">
-        <v>678</v>
+        <v>766</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -5998,22 +6807,22 @@
         <v>132</v>
       </c>
       <c r="D7" t="s">
-        <v>504</v>
+        <v>567</v>
       </c>
       <c r="E7" t="s">
-        <v>539</v>
+        <v>607</v>
       </c>
       <c r="F7" t="s">
-        <v>574</v>
+        <v>647</v>
       </c>
       <c r="G7" t="s">
-        <v>609</v>
+        <v>687</v>
       </c>
       <c r="H7" t="s">
-        <v>644</v>
+        <v>727</v>
       </c>
       <c r="I7" t="s">
-        <v>679</v>
+        <v>767</v>
       </c>
       <c r="J7">
         <v>6</v>
@@ -6045,22 +6854,22 @@
         <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>505</v>
+        <v>568</v>
       </c>
       <c r="E8" t="s">
-        <v>540</v>
+        <v>608</v>
       </c>
       <c r="F8" t="s">
-        <v>575</v>
+        <v>648</v>
       </c>
       <c r="G8" t="s">
-        <v>610</v>
+        <v>688</v>
       </c>
       <c r="H8" t="s">
-        <v>645</v>
+        <v>728</v>
       </c>
       <c r="I8" t="s">
-        <v>680</v>
+        <v>768</v>
       </c>
       <c r="J8">
         <v>7</v>
@@ -6092,22 +6901,22 @@
         <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>506</v>
+        <v>569</v>
       </c>
       <c r="E9" t="s">
-        <v>541</v>
+        <v>609</v>
       </c>
       <c r="F9" t="s">
-        <v>576</v>
+        <v>649</v>
       </c>
       <c r="G9" t="s">
-        <v>611</v>
+        <v>689</v>
       </c>
       <c r="H9" t="s">
-        <v>646</v>
+        <v>729</v>
       </c>
       <c r="I9" t="s">
-        <v>681</v>
+        <v>769</v>
       </c>
       <c r="J9">
         <v>8</v>
@@ -6139,22 +6948,22 @@
         <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>507</v>
+        <v>570</v>
       </c>
       <c r="E10" t="s">
-        <v>542</v>
+        <v>610</v>
       </c>
       <c r="F10" t="s">
-        <v>577</v>
+        <v>650</v>
       </c>
       <c r="G10" t="s">
-        <v>612</v>
+        <v>690</v>
       </c>
       <c r="H10" t="s">
-        <v>647</v>
+        <v>730</v>
       </c>
       <c r="I10" t="s">
-        <v>682</v>
+        <v>770</v>
       </c>
       <c r="J10">
         <v>9</v>
@@ -6186,22 +6995,22 @@
         <v>180</v>
       </c>
       <c r="D11" t="s">
-        <v>508</v>
+        <v>571</v>
       </c>
       <c r="E11" t="s">
-        <v>543</v>
+        <v>611</v>
       </c>
       <c r="F11" t="s">
-        <v>578</v>
+        <v>651</v>
       </c>
       <c r="G11" t="s">
-        <v>613</v>
+        <v>691</v>
       </c>
       <c r="H11" t="s">
-        <v>648</v>
+        <v>731</v>
       </c>
       <c r="I11" t="s">
-        <v>683</v>
+        <v>771</v>
       </c>
       <c r="J11">
         <v>10</v>
@@ -6233,22 +7042,22 @@
         <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>509</v>
+        <v>572</v>
       </c>
       <c r="E12" t="s">
-        <v>544</v>
+        <v>612</v>
       </c>
       <c r="F12" t="s">
-        <v>579</v>
+        <v>652</v>
       </c>
       <c r="G12" t="s">
-        <v>614</v>
+        <v>692</v>
       </c>
       <c r="H12" t="s">
-        <v>649</v>
+        <v>732</v>
       </c>
       <c r="I12" t="s">
-        <v>684</v>
+        <v>772</v>
       </c>
       <c r="J12">
         <v>11</v>
@@ -6280,22 +7089,22 @@
         <v>204</v>
       </c>
       <c r="D13" t="s">
-        <v>510</v>
+        <v>573</v>
       </c>
       <c r="E13" t="s">
-        <v>545</v>
+        <v>613</v>
       </c>
       <c r="F13" t="s">
-        <v>580</v>
+        <v>653</v>
       </c>
       <c r="G13" t="s">
-        <v>615</v>
+        <v>693</v>
       </c>
       <c r="H13" t="s">
-        <v>650</v>
+        <v>733</v>
       </c>
       <c r="I13" t="s">
-        <v>685</v>
+        <v>773</v>
       </c>
       <c r="J13">
         <v>12</v>
@@ -6327,22 +7136,22 @@
         <v>216</v>
       </c>
       <c r="D14" t="s">
-        <v>511</v>
+        <v>574</v>
       </c>
       <c r="E14" t="s">
-        <v>546</v>
+        <v>614</v>
       </c>
       <c r="F14" t="s">
-        <v>581</v>
+        <v>654</v>
       </c>
       <c r="G14" t="s">
-        <v>616</v>
+        <v>694</v>
       </c>
       <c r="H14" t="s">
-        <v>651</v>
+        <v>734</v>
       </c>
       <c r="I14" t="s">
-        <v>686</v>
+        <v>774</v>
       </c>
       <c r="J14">
         <v>13</v>
@@ -6374,22 +7183,22 @@
         <v>226</v>
       </c>
       <c r="D15" t="s">
-        <v>512</v>
+        <v>575</v>
       </c>
       <c r="E15" t="s">
-        <v>547</v>
+        <v>615</v>
       </c>
       <c r="F15" t="s">
-        <v>582</v>
+        <v>655</v>
       </c>
       <c r="G15" t="s">
-        <v>617</v>
+        <v>695</v>
       </c>
       <c r="H15" t="s">
-        <v>652</v>
+        <v>735</v>
       </c>
       <c r="I15" t="s">
-        <v>687</v>
+        <v>775</v>
       </c>
       <c r="J15">
         <v>14</v>
@@ -6421,22 +7230,22 @@
         <v>237</v>
       </c>
       <c r="D16" t="s">
-        <v>513</v>
+        <v>576</v>
       </c>
       <c r="E16" t="s">
-        <v>548</v>
+        <v>616</v>
       </c>
       <c r="F16" t="s">
-        <v>583</v>
+        <v>656</v>
       </c>
       <c r="G16" t="s">
-        <v>618</v>
+        <v>696</v>
       </c>
       <c r="H16" t="s">
-        <v>653</v>
+        <v>736</v>
       </c>
       <c r="I16" t="s">
-        <v>688</v>
+        <v>776</v>
       </c>
       <c r="J16">
         <v>15</v>
@@ -6468,22 +7277,22 @@
         <v>249</v>
       </c>
       <c r="D17" t="s">
-        <v>514</v>
+        <v>577</v>
       </c>
       <c r="E17" t="s">
-        <v>549</v>
+        <v>617</v>
       </c>
       <c r="F17" t="s">
-        <v>584</v>
+        <v>657</v>
       </c>
       <c r="G17" t="s">
-        <v>619</v>
+        <v>697</v>
       </c>
       <c r="H17" t="s">
-        <v>654</v>
+        <v>737</v>
       </c>
       <c r="I17" t="s">
-        <v>689</v>
+        <v>777</v>
       </c>
       <c r="J17">
         <v>16</v>
@@ -6515,22 +7324,22 @@
         <v>261</v>
       </c>
       <c r="D18" t="s">
-        <v>515</v>
+        <v>578</v>
       </c>
       <c r="E18" t="s">
-        <v>550</v>
+        <v>618</v>
       </c>
       <c r="F18" t="s">
-        <v>585</v>
+        <v>658</v>
       </c>
       <c r="G18" t="s">
-        <v>620</v>
+        <v>698</v>
       </c>
       <c r="H18" t="s">
-        <v>655</v>
+        <v>738</v>
       </c>
       <c r="I18" t="s">
-        <v>690</v>
+        <v>778</v>
       </c>
       <c r="J18">
         <v>17</v>
@@ -6562,22 +7371,22 @@
         <v>266</v>
       </c>
       <c r="D19" t="s">
-        <v>516</v>
+        <v>579</v>
       </c>
       <c r="E19" t="s">
-        <v>551</v>
+        <v>619</v>
       </c>
       <c r="F19" t="s">
-        <v>586</v>
+        <v>659</v>
       </c>
       <c r="G19" t="s">
-        <v>621</v>
+        <v>699</v>
       </c>
       <c r="H19" t="s">
-        <v>656</v>
+        <v>739</v>
       </c>
       <c r="I19" t="s">
-        <v>691</v>
+        <v>779</v>
       </c>
       <c r="J19">
         <v>18</v>
@@ -6609,22 +7418,22 @@
         <v>273</v>
       </c>
       <c r="D20" t="s">
-        <v>517</v>
+        <v>580</v>
       </c>
       <c r="E20" t="s">
-        <v>552</v>
+        <v>620</v>
       </c>
       <c r="F20" t="s">
-        <v>587</v>
+        <v>660</v>
       </c>
       <c r="G20" t="s">
-        <v>622</v>
+        <v>700</v>
       </c>
       <c r="H20" t="s">
-        <v>657</v>
+        <v>740</v>
       </c>
       <c r="I20" t="s">
-        <v>692</v>
+        <v>780</v>
       </c>
       <c r="J20">
         <v>19</v>
@@ -6656,22 +7465,22 @@
         <v>286</v>
       </c>
       <c r="D21" t="s">
-        <v>518</v>
+        <v>581</v>
       </c>
       <c r="E21" t="s">
-        <v>553</v>
+        <v>621</v>
       </c>
       <c r="F21" t="s">
-        <v>588</v>
+        <v>661</v>
       </c>
       <c r="G21" t="s">
-        <v>623</v>
+        <v>701</v>
       </c>
       <c r="H21" t="s">
-        <v>658</v>
+        <v>741</v>
       </c>
       <c r="I21" t="s">
-        <v>693</v>
+        <v>781</v>
       </c>
       <c r="J21">
         <v>20</v>
@@ -6703,22 +7512,22 @@
         <v>298</v>
       </c>
       <c r="D22" t="s">
-        <v>519</v>
+        <v>582</v>
       </c>
       <c r="E22" t="s">
-        <v>554</v>
+        <v>622</v>
       </c>
       <c r="F22" t="s">
-        <v>589</v>
+        <v>662</v>
       </c>
       <c r="G22" t="s">
-        <v>624</v>
+        <v>702</v>
       </c>
       <c r="H22" t="s">
-        <v>659</v>
+        <v>742</v>
       </c>
       <c r="I22" t="s">
-        <v>694</v>
+        <v>782</v>
       </c>
       <c r="J22">
         <v>21</v>
@@ -6750,22 +7559,22 @@
         <v>310</v>
       </c>
       <c r="D23" t="s">
-        <v>520</v>
+        <v>583</v>
       </c>
       <c r="E23" t="s">
-        <v>555</v>
+        <v>623</v>
       </c>
       <c r="F23" t="s">
-        <v>590</v>
+        <v>663</v>
       </c>
       <c r="G23" t="s">
-        <v>625</v>
+        <v>703</v>
       </c>
       <c r="H23" t="s">
-        <v>660</v>
+        <v>743</v>
       </c>
       <c r="I23" t="s">
-        <v>695</v>
+        <v>783</v>
       </c>
       <c r="J23">
         <v>22</v>
@@ -6797,22 +7606,22 @@
         <v>318</v>
       </c>
       <c r="D24" t="s">
-        <v>521</v>
+        <v>584</v>
       </c>
       <c r="E24" t="s">
-        <v>556</v>
+        <v>624</v>
       </c>
       <c r="F24" t="s">
-        <v>591</v>
+        <v>664</v>
       </c>
       <c r="G24" t="s">
-        <v>626</v>
+        <v>704</v>
       </c>
       <c r="H24" t="s">
-        <v>661</v>
+        <v>744</v>
       </c>
       <c r="I24" t="s">
-        <v>696</v>
+        <v>784</v>
       </c>
       <c r="J24">
         <v>23</v>
@@ -6844,22 +7653,22 @@
         <v>332</v>
       </c>
       <c r="D25" t="s">
-        <v>522</v>
+        <v>585</v>
       </c>
       <c r="E25" t="s">
-        <v>557</v>
+        <v>625</v>
       </c>
       <c r="F25" t="s">
-        <v>592</v>
+        <v>665</v>
       </c>
       <c r="G25" t="s">
-        <v>627</v>
+        <v>705</v>
       </c>
       <c r="H25" t="s">
-        <v>662</v>
+        <v>745</v>
       </c>
       <c r="I25" t="s">
-        <v>697</v>
+        <v>785</v>
       </c>
       <c r="J25">
         <v>24</v>
@@ -6891,22 +7700,22 @@
         <v>339</v>
       </c>
       <c r="D26" t="s">
-        <v>523</v>
+        <v>586</v>
       </c>
       <c r="E26" t="s">
-        <v>558</v>
+        <v>626</v>
       </c>
       <c r="F26" t="s">
-        <v>593</v>
+        <v>666</v>
       </c>
       <c r="G26" t="s">
-        <v>628</v>
+        <v>706</v>
       </c>
       <c r="H26" t="s">
-        <v>663</v>
+        <v>746</v>
       </c>
       <c r="I26" t="s">
-        <v>698</v>
+        <v>786</v>
       </c>
       <c r="J26">
         <v>25</v>
@@ -6938,22 +7747,22 @@
         <v>339</v>
       </c>
       <c r="D27" t="s">
-        <v>523</v>
+        <v>586</v>
       </c>
       <c r="E27" t="s">
-        <v>558</v>
+        <v>626</v>
       </c>
       <c r="F27" t="s">
-        <v>593</v>
+        <v>666</v>
       </c>
       <c r="G27" t="s">
-        <v>628</v>
+        <v>706</v>
       </c>
       <c r="H27" t="s">
-        <v>663</v>
+        <v>746</v>
       </c>
       <c r="I27" t="s">
-        <v>698</v>
+        <v>786</v>
       </c>
       <c r="J27">
         <v>25</v>
@@ -6985,22 +7794,22 @@
         <v>349</v>
       </c>
       <c r="D28" t="s">
-        <v>524</v>
+        <v>587</v>
       </c>
       <c r="E28" t="s">
-        <v>559</v>
+        <v>627</v>
       </c>
       <c r="F28" t="s">
-        <v>594</v>
+        <v>667</v>
       </c>
       <c r="G28" t="s">
-        <v>629</v>
+        <v>707</v>
       </c>
       <c r="H28" t="s">
-        <v>664</v>
+        <v>747</v>
       </c>
       <c r="I28" t="s">
-        <v>699</v>
+        <v>787</v>
       </c>
       <c r="J28">
         <v>26</v>
@@ -7032,22 +7841,22 @@
         <v>362</v>
       </c>
       <c r="D29" t="s">
-        <v>525</v>
+        <v>588</v>
       </c>
       <c r="E29" t="s">
-        <v>560</v>
+        <v>628</v>
       </c>
       <c r="F29" t="s">
-        <v>595</v>
+        <v>668</v>
       </c>
       <c r="G29" t="s">
-        <v>630</v>
+        <v>708</v>
       </c>
       <c r="H29" t="s">
-        <v>665</v>
+        <v>748</v>
       </c>
       <c r="I29" t="s">
-        <v>700</v>
+        <v>788</v>
       </c>
       <c r="J29">
         <v>27</v>
@@ -7079,22 +7888,22 @@
         <v>375</v>
       </c>
       <c r="D30" t="s">
-        <v>526</v>
+        <v>589</v>
       </c>
       <c r="E30" t="s">
-        <v>561</v>
+        <v>629</v>
       </c>
       <c r="F30" t="s">
-        <v>596</v>
+        <v>669</v>
       </c>
       <c r="G30" t="s">
-        <v>631</v>
+        <v>709</v>
       </c>
       <c r="H30" t="s">
-        <v>666</v>
+        <v>749</v>
       </c>
       <c r="I30" t="s">
-        <v>701</v>
+        <v>789</v>
       </c>
       <c r="J30">
         <v>28</v>
@@ -7126,22 +7935,22 @@
         <v>388</v>
       </c>
       <c r="D31" t="s">
-        <v>527</v>
+        <v>590</v>
       </c>
       <c r="E31" t="s">
-        <v>562</v>
+        <v>630</v>
       </c>
       <c r="F31" t="s">
-        <v>597</v>
+        <v>670</v>
       </c>
       <c r="G31" t="s">
-        <v>632</v>
+        <v>710</v>
       </c>
       <c r="H31" t="s">
-        <v>667</v>
+        <v>750</v>
       </c>
       <c r="I31" t="s">
-        <v>702</v>
+        <v>790</v>
       </c>
       <c r="J31">
         <v>29</v>
@@ -7173,22 +7982,22 @@
         <v>397</v>
       </c>
       <c r="D32" t="s">
-        <v>528</v>
+        <v>591</v>
       </c>
       <c r="E32" t="s">
-        <v>563</v>
+        <v>631</v>
       </c>
       <c r="F32" t="s">
-        <v>598</v>
+        <v>671</v>
       </c>
       <c r="G32" t="s">
-        <v>633</v>
+        <v>711</v>
       </c>
       <c r="H32" t="s">
-        <v>668</v>
+        <v>751</v>
       </c>
       <c r="I32" t="s">
-        <v>703</v>
+        <v>791</v>
       </c>
       <c r="J32">
         <v>30</v>
@@ -7220,22 +8029,22 @@
         <v>406</v>
       </c>
       <c r="D33" t="s">
-        <v>529</v>
+        <v>592</v>
       </c>
       <c r="E33" t="s">
-        <v>564</v>
+        <v>632</v>
       </c>
       <c r="F33" t="s">
-        <v>599</v>
+        <v>672</v>
       </c>
       <c r="G33" t="s">
-        <v>634</v>
+        <v>712</v>
       </c>
       <c r="H33" t="s">
-        <v>669</v>
+        <v>752</v>
       </c>
       <c r="I33" t="s">
-        <v>704</v>
+        <v>792</v>
       </c>
       <c r="J33">
         <v>31</v>
@@ -7267,22 +8076,22 @@
         <v>419</v>
       </c>
       <c r="D34" t="s">
-        <v>530</v>
+        <v>593</v>
       </c>
       <c r="E34" t="s">
-        <v>565</v>
+        <v>633</v>
       </c>
       <c r="F34" t="s">
-        <v>600</v>
+        <v>673</v>
       </c>
       <c r="G34" t="s">
-        <v>635</v>
+        <v>713</v>
       </c>
       <c r="H34" t="s">
-        <v>670</v>
+        <v>753</v>
       </c>
       <c r="I34" t="s">
-        <v>705</v>
+        <v>793</v>
       </c>
       <c r="J34">
         <v>32</v>
@@ -7314,22 +8123,22 @@
         <v>419</v>
       </c>
       <c r="D35" t="s">
-        <v>530</v>
+        <v>593</v>
       </c>
       <c r="E35" t="s">
-        <v>565</v>
+        <v>633</v>
       </c>
       <c r="F35" t="s">
-        <v>600</v>
+        <v>673</v>
       </c>
       <c r="G35" t="s">
-        <v>635</v>
+        <v>713</v>
       </c>
       <c r="H35" t="s">
-        <v>670</v>
+        <v>753</v>
       </c>
       <c r="I35" t="s">
-        <v>705</v>
+        <v>793</v>
       </c>
       <c r="J35">
         <v>32</v>
@@ -7361,22 +8170,22 @@
         <v>434</v>
       </c>
       <c r="D36" t="s">
-        <v>531</v>
+        <v>594</v>
       </c>
       <c r="E36" t="s">
-        <v>566</v>
+        <v>634</v>
       </c>
       <c r="F36" t="s">
-        <v>601</v>
+        <v>674</v>
       </c>
       <c r="G36" t="s">
-        <v>636</v>
+        <v>714</v>
       </c>
       <c r="H36" t="s">
-        <v>671</v>
+        <v>754</v>
       </c>
       <c r="I36" t="s">
-        <v>706</v>
+        <v>794</v>
       </c>
       <c r="J36">
         <v>33</v>
@@ -7408,22 +8217,22 @@
         <v>447</v>
       </c>
       <c r="D37" t="s">
-        <v>532</v>
+        <v>595</v>
       </c>
       <c r="E37" t="s">
-        <v>567</v>
+        <v>635</v>
       </c>
       <c r="F37" t="s">
-        <v>602</v>
+        <v>675</v>
       </c>
       <c r="G37" t="s">
-        <v>637</v>
+        <v>715</v>
       </c>
       <c r="H37" t="s">
-        <v>672</v>
+        <v>755</v>
       </c>
       <c r="I37" t="s">
-        <v>707</v>
+        <v>795</v>
       </c>
       <c r="J37">
         <v>34</v>
@@ -7455,22 +8264,22 @@
         <v>460</v>
       </c>
       <c r="D38" t="s">
-        <v>533</v>
+        <v>596</v>
       </c>
       <c r="E38" t="s">
-        <v>568</v>
+        <v>636</v>
       </c>
       <c r="F38" t="s">
-        <v>603</v>
+        <v>676</v>
       </c>
       <c r="G38" t="s">
-        <v>638</v>
+        <v>716</v>
       </c>
       <c r="H38" t="s">
-        <v>673</v>
+        <v>756</v>
       </c>
       <c r="I38" t="s">
-        <v>708</v>
+        <v>796</v>
       </c>
       <c r="J38">
         <v>35</v>
@@ -7482,13 +8291,295 @@
         <v>1.1472027099550692</v>
       </c>
       <c r="M38">
-        <v>1.1341092724704294</v>
+        <v>1.165801686137024</v>
       </c>
       <c r="N38">
-        <v>3580</v>
+        <v>3708</v>
       </c>
       <c r="O38">
-        <v>2991.5</v>
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1">
+        <v>45876</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>474</v>
+      </c>
+      <c r="D39" t="s">
+        <v>597</v>
+      </c>
+      <c r="E39" t="s">
+        <v>637</v>
+      </c>
+      <c r="F39" t="s">
+        <v>677</v>
+      </c>
+      <c r="G39" t="s">
+        <v>717</v>
+      </c>
+      <c r="H39" t="s">
+        <v>757</v>
+      </c>
+      <c r="I39" t="s">
+        <v>797</v>
+      </c>
+      <c r="J39">
+        <v>36</v>
+      </c>
+      <c r="K39">
+        <v>115.6668776371308</v>
+      </c>
+      <c r="L39">
+        <v>1.1465507707023657</v>
+      </c>
+      <c r="M39">
+        <v>1.1634922651375534</v>
+      </c>
+      <c r="N39">
+        <v>3845</v>
+      </c>
+      <c r="O39">
+        <v>3173</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1">
+        <v>45877</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>488</v>
+      </c>
+      <c r="D40" t="s">
+        <v>598</v>
+      </c>
+      <c r="E40" t="s">
+        <v>638</v>
+      </c>
+      <c r="F40" t="s">
+        <v>678</v>
+      </c>
+      <c r="G40" t="s">
+        <v>718</v>
+      </c>
+      <c r="H40" t="s">
+        <v>758</v>
+      </c>
+      <c r="I40" t="s">
+        <v>798</v>
+      </c>
+      <c r="J40">
+        <v>37</v>
+      </c>
+      <c r="K40">
+        <v>116.25188524590163</v>
+      </c>
+      <c r="L40">
+        <v>1.1455884999883459</v>
+      </c>
+      <c r="M40">
+        <v>1.161409079625294</v>
+      </c>
+      <c r="N40">
+        <v>3981</v>
+      </c>
+      <c r="O40">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1">
+        <v>45878</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>488</v>
+      </c>
+      <c r="D41" t="s">
+        <v>598</v>
+      </c>
+      <c r="E41" t="s">
+        <v>638</v>
+      </c>
+      <c r="F41" t="s">
+        <v>678</v>
+      </c>
+      <c r="G41" t="s">
+        <v>718</v>
+      </c>
+      <c r="H41" t="s">
+        <v>758</v>
+      </c>
+      <c r="I41" t="s">
+        <v>798</v>
+      </c>
+      <c r="J41">
+        <v>37</v>
+      </c>
+      <c r="K41">
+        <v>116.25188524590163</v>
+      </c>
+      <c r="L41">
+        <v>1.1455884999883459</v>
+      </c>
+      <c r="M41">
+        <v>1.161409079625294</v>
+      </c>
+      <c r="N41">
+        <v>3981</v>
+      </c>
+      <c r="O41">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1">
+        <v>45880</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>500</v>
+      </c>
+      <c r="D42" t="s">
+        <v>599</v>
+      </c>
+      <c r="E42" t="s">
+        <v>639</v>
+      </c>
+      <c r="F42" t="s">
+        <v>679</v>
+      </c>
+      <c r="G42" t="s">
+        <v>719</v>
+      </c>
+      <c r="H42" t="s">
+        <v>759</v>
+      </c>
+      <c r="I42" t="s">
+        <v>799</v>
+      </c>
+      <c r="J42">
+        <v>38</v>
+      </c>
+      <c r="K42">
+        <v>116.65181999999999</v>
+      </c>
+      <c r="L42">
+        <v>1.1456172138523208</v>
+      </c>
+      <c r="M42">
+        <v>1.1615834279371564</v>
+      </c>
+      <c r="N42">
+        <v>4103</v>
+      </c>
+      <c r="O42">
+        <v>3343.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>45881</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>513</v>
+      </c>
+      <c r="D43" t="s">
+        <v>600</v>
+      </c>
+      <c r="E43" t="s">
+        <v>640</v>
+      </c>
+      <c r="F43" t="s">
+        <v>680</v>
+      </c>
+      <c r="G43" t="s">
+        <v>720</v>
+      </c>
+      <c r="H43" t="s">
+        <v>760</v>
+      </c>
+      <c r="I43" t="s">
+        <v>800</v>
+      </c>
+      <c r="J43">
+        <v>39</v>
+      </c>
+      <c r="K43">
+        <v>117.16411306042885</v>
+      </c>
+      <c r="L43">
+        <v>1.144904060343408</v>
+      </c>
+      <c r="M43">
+        <v>1.1600012989673765</v>
+      </c>
+      <c r="N43">
+        <v>4231</v>
+      </c>
+      <c r="O43">
+        <v>3434</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1">
+        <v>45882</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>524</v>
+      </c>
+      <c r="D44" t="s">
+        <v>601</v>
+      </c>
+      <c r="E44" t="s">
+        <v>641</v>
+      </c>
+      <c r="F44" t="s">
+        <v>681</v>
+      </c>
+      <c r="G44" t="s">
+        <v>721</v>
+      </c>
+      <c r="H44" t="s">
+        <v>761</v>
+      </c>
+      <c r="I44" t="s">
+        <v>801</v>
+      </c>
+      <c r="J44">
+        <v>40</v>
+      </c>
+      <c r="K44">
+        <v>117.5028816793893</v>
+      </c>
+      <c r="L44">
+        <v>1.1442336455639506</v>
+      </c>
+      <c r="M44">
+        <v>1.1636485756885324</v>
+      </c>
+      <c r="N44">
+        <v>4359</v>
+      </c>
+      <c r="O44">
+        <v>3517.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>